<commit_message>
update notes of phase 6 of bomb of CSAPP 3e
</commit_message>
<xml_diff>
--- a/CSAPP/labs/labs_of_CSAPP3e/2_Bomb_Lab/bomb/stack frame of phase 6 of bomb.xlsx
+++ b/CSAPP/labs/labs_of_CSAPP3e/2_Bomb_Lab/bomb/stack frame of phase 6 of bomb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>0x14(%rsp)</t>
   </si>
@@ -96,9 +96,6 @@
     <t>phase_6(...)</t>
   </si>
   <si>
-    <t>Before executing "0x40116f"</t>
-  </si>
-  <si>
     <t>0x28(%rsp)</t>
   </si>
   <si>
@@ -117,20 +114,38 @@
     <t>After executing 0x401195, the current is as above</t>
   </si>
   <si>
-    <t>4 bytes eacg row</t>
-  </si>
-  <si>
     <t>When the instructions from 0x40116f to 0x4011a9 are executed, the state of memory is as follows:</t>
   </si>
   <si>
     <t>0x603328</t>
+  </si>
+  <si>
+    <t>at 0x4011c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the first loop, </t>
+  </si>
+  <si>
+    <t>The array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illustration of the 4th step of my note of phase 6. </t>
+  </si>
+  <si>
+    <t>Step 3 of my note. Before executing "0x40116f"</t>
+  </si>
+  <si>
+    <t>4 bytes each row</t>
+  </si>
+  <si>
+    <t>After 0x4011cb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +161,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -212,11 +250,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,15 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -260,6 +320,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,96 +652,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:Q34"/>
+  <dimension ref="E1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="I1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="20"/>
     </row>
     <row r="2" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -661,16 +769,17 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -690,7 +799,9 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="M8" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
@@ -704,18 +815,18 @@
         <v>18</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
+      <c r="M9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="14"/>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
@@ -732,15 +843,17 @@
       <c r="N10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="14" t="s">
-        <v>32</v>
+      <c r="G11" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>21</v>
@@ -757,7 +870,9 @@
       <c r="N11" s="3">
         <v>332</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="3">
+        <v>1</v>
+      </c>
       <c r="P11" s="4" t="s">
         <v>13</v>
       </c>
@@ -783,8 +898,8 @@
     <row r="13" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="12" t="s">
-        <v>26</v>
+      <c r="G13" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -802,6 +917,7 @@
         <v>8</v>
       </c>
       <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="5:17" x14ac:dyDescent="0.25">
@@ -826,7 +942,9 @@
     <row r="15" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="3">
         <v>2</v>
       </c>
@@ -840,7 +958,9 @@
       <c r="N15" s="3">
         <v>168</v>
       </c>
-      <c r="O15" s="3"/>
+      <c r="O15" s="3">
+        <v>2</v>
+      </c>
       <c r="P15" s="4" t="s">
         <v>11</v>
       </c>
@@ -881,6 +1001,7 @@
         <v>10</v>
       </c>
       <c r="O17" s="3"/>
+      <c r="P17" s="4"/>
       <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
@@ -891,9 +1012,6 @@
         <v>5</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -923,7 +1041,9 @@
       <c r="N19" s="3">
         <v>924</v>
       </c>
-      <c r="O19" s="3"/>
+      <c r="O19" s="3">
+        <v>3</v>
+      </c>
       <c r="P19" s="4" t="s">
         <v>12</v>
       </c>
@@ -960,6 +1080,7 @@
         <v>15</v>
       </c>
       <c r="O21" s="3"/>
+      <c r="P21" s="4"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="5:17" x14ac:dyDescent="0.25">
@@ -992,7 +1113,9 @@
       <c r="N23" s="3">
         <v>691</v>
       </c>
-      <c r="O23" s="3"/>
+      <c r="O23" s="3">
+        <v>4</v>
+      </c>
       <c r="P23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1029,6 +1152,7 @@
         <v>18</v>
       </c>
       <c r="O25" s="3"/>
+      <c r="P25" s="4"/>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="5:17" x14ac:dyDescent="0.25">
@@ -1061,7 +1185,9 @@
       <c r="N27" s="3">
         <v>477</v>
       </c>
-      <c r="O27" s="3"/>
+      <c r="O27" s="3">
+        <v>5</v>
+      </c>
       <c r="P27" s="4" t="s">
         <v>19</v>
       </c>
@@ -1098,6 +1224,7 @@
         <v>21</v>
       </c>
       <c r="O29" s="3"/>
+      <c r="P29" s="4"/>
       <c r="Q29" s="5"/>
     </row>
     <row r="30" spans="5:17" x14ac:dyDescent="0.25">
@@ -1130,7 +1257,9 @@
       <c r="N31" s="3">
         <v>443</v>
       </c>
-      <c r="O31" s="3"/>
+      <c r="O31" s="3">
+        <v>6</v>
+      </c>
       <c r="P31" s="4" t="s">
         <v>22</v>
       </c>
@@ -1157,15 +1286,11 @@
       <c r="G33" s="2"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="M33" s="11"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="5"/>
@@ -1184,6 +1309,255 @@
       <c r="O34" s="7"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="9"/>
+    </row>
+    <row r="38" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M38" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="14"/>
+    </row>
+    <row r="39" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="3"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N40" s="3">
+        <v>332</v>
+      </c>
+      <c r="O40" s="3"/>
+      <c r="P40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" s="16">
+        <v>0</v>
+      </c>
+      <c r="O42" s="3"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" s="3">
+        <v>168</v>
+      </c>
+      <c r="O44" s="3"/>
+      <c r="P44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O46" s="3"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" s="3">
+        <v>924</v>
+      </c>
+      <c r="O48" s="3"/>
+      <c r="P48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O50" s="3"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N52" s="3">
+        <v>691</v>
+      </c>
+      <c r="O52" s="3"/>
+      <c r="P52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" s="3"/>
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N56" s="3">
+        <v>477</v>
+      </c>
+      <c r="O56" s="3"/>
+      <c r="P56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q56" s="5"/>
+    </row>
+    <row r="57" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="5"/>
+    </row>
+    <row r="58" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N58" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O58" s="3"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="5"/>
+    </row>
+    <row r="60" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M60" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" s="3">
+        <v>443</v>
+      </c>
+      <c r="O60" s="3"/>
+      <c r="P60" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q60" s="5"/>
+    </row>
+    <row r="61" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="5"/>
+    </row>
+    <row r="62" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J62" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M62" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N62" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="O62" s="3"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="5"/>
+    </row>
+    <row r="63" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>